<commit_message>
Added more mgaye files, added percentage profile
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -13,10 +13,6 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -346,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:D8"/>
+  <dimension ref="A3:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -357,40 +353,66 @@
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="B3">
-        <v>1500</v>
+        <v>0.2</v>
       </c>
       <c r="C3">
-        <v>2000</v>
+        <v>0.4</v>
       </c>
       <c r="D3">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.6</v>
+      </c>
+      <c r="E3">
+        <v>0.8</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filling out table of results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="5">
   <si>
     <t>BL--Rthicke</t>
   </si>
@@ -29,12 +29,15 @@
   <si>
     <t>Original-Mgaye</t>
   </si>
+  <si>
+    <t>(%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,8 +45,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -53,6 +64,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -69,15 +86,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,168 +394,969 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:U12"/>
+  <dimension ref="A2:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="9.140625" style="3"/>
+    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:21">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="B3" s="2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6">
         <v>0.2</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7">
         <v>0.4</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="6">
         <v>0.6</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="1">
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="7">
         <v>0.8</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="2">
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="6">
         <v>1</v>
       </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3.22</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.57</v>
+      </c>
+      <c r="F4" s="5">
+        <v>35.1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>23.59</v>
+      </c>
+      <c r="H4" s="4">
+        <v>12.56</v>
+      </c>
+      <c r="I4" s="5">
+        <v>32.76</v>
+      </c>
+      <c r="J4" s="2">
+        <v>71.09</v>
+      </c>
+      <c r="K4" s="2">
+        <v>52.73</v>
+      </c>
+      <c r="L4" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="M4" s="2">
+        <v>83.73</v>
+      </c>
+      <c r="N4" s="5">
+        <v>138.07</v>
+      </c>
+      <c r="O4" s="5">
+        <v>103.88</v>
+      </c>
+      <c r="P4" s="4">
+        <v>50.23</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>145.69999999999999</v>
+      </c>
+      <c r="R4" s="2">
+        <v>159.13999999999999</v>
+      </c>
+      <c r="S4" s="2">
+        <v>140.43</v>
+      </c>
+      <c r="T4" s="3">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="U4" s="2">
+        <v>180.97</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>55.01</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43.34</v>
+      </c>
+      <c r="D5" s="4">
+        <v>36.56</v>
+      </c>
+      <c r="E5" s="2">
+        <v>53.09</v>
+      </c>
+      <c r="F5" s="5">
+        <v>243.25</v>
+      </c>
+      <c r="G5" s="4">
+        <v>212.01</v>
+      </c>
+      <c r="H5" s="5">
+        <v>214.58</v>
+      </c>
+      <c r="I5" s="5">
+        <v>251.64</v>
+      </c>
+      <c r="J5" s="2">
+        <v>538</v>
+      </c>
+      <c r="K5" s="2">
+        <v>429.73</v>
+      </c>
+      <c r="L5" s="4">
+        <v>367.36</v>
+      </c>
+      <c r="M5" s="2">
+        <v>595.17999999999995</v>
+      </c>
+      <c r="N5" s="5">
+        <v>911.94</v>
+      </c>
+      <c r="O5" s="5">
+        <v>781.26</v>
+      </c>
+      <c r="P5" s="4">
+        <v>646.87</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>974.24</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1119.98</v>
+      </c>
+      <c r="S5" s="2">
+        <v>899.8</v>
+      </c>
+      <c r="T5" s="4">
+        <v>785.51</v>
+      </c>
+      <c r="U5" s="2">
+        <v>1180.93</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>132.02000000000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>124.49</v>
+      </c>
+      <c r="D6" s="2">
+        <v>134.35</v>
+      </c>
+      <c r="E6" s="2">
+        <v>135.78</v>
+      </c>
+      <c r="F6" s="5">
+        <v>603.16999999999996</v>
+      </c>
+      <c r="G6" s="4">
+        <v>549.15</v>
+      </c>
+      <c r="H6" s="5">
+        <v>591.42999999999995</v>
+      </c>
+      <c r="I6" s="5">
+        <v>665.77</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1535.25</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1347.98</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1366.89</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1547</v>
+      </c>
+      <c r="N6" s="5">
+        <v>2538.87</v>
+      </c>
+      <c r="O6" s="5">
+        <v>2260.73</v>
+      </c>
+      <c r="P6" s="4">
+        <v>2385.98</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>2590.6799999999998</v>
+      </c>
+      <c r="R6" s="2">
+        <v>3070.2</v>
+      </c>
+      <c r="S6" s="2">
+        <v>2819.98</v>
+      </c>
+      <c r="T6" s="4">
+        <v>2787.74</v>
+      </c>
+      <c r="U6" s="2">
+        <v>3091.91</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>204.29</v>
+      </c>
+      <c r="C7" s="4">
+        <v>185.37</v>
+      </c>
+      <c r="D7" s="2">
+        <v>225.89</v>
+      </c>
+      <c r="E7" s="2">
+        <v>222.77</v>
+      </c>
+      <c r="F7" s="5">
+        <v>941.63</v>
+      </c>
+      <c r="G7" s="4">
+        <v>834.43</v>
+      </c>
+      <c r="H7" s="5">
+        <v>908.28</v>
+      </c>
+      <c r="I7" s="5">
+        <v>955.48</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2439.79</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2235.62</v>
+      </c>
+      <c r="L7" s="2">
+        <v>2468.77</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2447.44</v>
+      </c>
+      <c r="N7" s="5">
+        <v>3991.14</v>
+      </c>
+      <c r="O7" s="4">
+        <v>3734.55</v>
+      </c>
+      <c r="P7" s="8">
+        <v>4021.34</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>3883.76</v>
+      </c>
+      <c r="R7" s="2">
+        <v>4720.2</v>
+      </c>
+      <c r="S7" s="2">
+        <v>4857.7</v>
+      </c>
+      <c r="T7" s="4">
+        <v>4681.33</v>
+      </c>
+      <c r="U7" s="2">
+        <v>4976.71</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="2">
+        <v>6205.06</v>
+      </c>
+      <c r="S8" s="4">
+        <v>5895.71</v>
+      </c>
+      <c r="T8" s="2">
+        <v>6224.36</v>
+      </c>
+      <c r="U8" s="2">
+        <v>5898.08</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
     </row>
     <row r="10" spans="1:21">
       <c r="A10">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
     </row>
     <row r="11" spans="1:21">
       <c r="A11">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
     </row>
     <row r="12" spans="1:21">
       <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13">
         <v>10</v>
       </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="2:21">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18" spans="2:21">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="2:21">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+    </row>
+    <row r="20" spans="2:21">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="2:21">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="2:21">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="2:21">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="2:21">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="2:21">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="2:21">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="2:21">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+    </row>
+    <row r="28" spans="2:21">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+    </row>
+    <row r="29" spans="2:21">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30" spans="2:21">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="2:21">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="2:21">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Finished collecting results for ngrams with size 8
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="21075" windowHeight="8250"/>
+    <workbookView xWindow="-60" yWindow="-20" windowWidth="38020" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -36,8 +41,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,7 +59,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +78,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -86,20 +97,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,36 +405,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:21">
@@ -491,36 +503,36 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>0.2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8">
         <v>0.4</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="6">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="7">
         <v>0.6</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="7">
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="8">
         <v>0.8</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="6">
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="7">
         <v>1</v>
       </c>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4">
@@ -616,7 +628,7 @@
         <v>251.64</v>
       </c>
       <c r="J5" s="2">
-        <v>538</v>
+        <v>535.02</v>
       </c>
       <c r="K5" s="2">
         <v>429.73</v>
@@ -763,7 +775,7 @@
       <c r="O7" s="4">
         <v>3734.55</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="6">
         <v>4021.34</v>
       </c>
       <c r="Q7" s="5">
@@ -786,22 +798,54 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
+      <c r="B8" s="2">
+        <v>240.49</v>
+      </c>
+      <c r="C8" s="9">
+        <v>231.17</v>
+      </c>
+      <c r="D8" s="2">
+        <v>257.92</v>
+      </c>
+      <c r="E8" s="2">
+        <v>253.47</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1168.83</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1062.18</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1144.1199999999999</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1202.8800000000001</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2987.73</v>
+      </c>
+      <c r="K8" s="9">
+        <v>2875.32</v>
+      </c>
+      <c r="L8" s="2">
+        <v>3083.99</v>
+      </c>
+      <c r="M8" s="2">
+        <v>2996.66</v>
+      </c>
+      <c r="N8" s="5">
+        <v>4910.5200000000004</v>
+      </c>
+      <c r="O8" s="9">
+        <v>4741.32</v>
+      </c>
+      <c r="P8" s="6">
+        <v>5048.5</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>4774.8500000000004</v>
+      </c>
       <c r="R8" s="2">
         <v>6205.06</v>
       </c>
@@ -819,76 +863,196 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="B9" s="2">
+        <v>268.05</v>
+      </c>
+      <c r="C9" s="2">
+        <v>265.73</v>
+      </c>
+      <c r="D9" s="2">
+        <v>280</v>
+      </c>
+      <c r="E9" s="2">
+        <v>280</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1342.79</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1310.82</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1353.5</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1348.58</v>
+      </c>
+      <c r="J9" s="2">
+        <v>3415.66</v>
+      </c>
+      <c r="K9" s="9">
+        <v>3227.09</v>
+      </c>
+      <c r="L9" s="2">
+        <v>3466.5</v>
+      </c>
+      <c r="M9" s="2">
+        <v>3359.1</v>
+      </c>
+      <c r="N9" s="5">
+        <v>5584.42</v>
+      </c>
+      <c r="O9" s="9">
+        <v>5370.85</v>
+      </c>
+      <c r="P9" s="6">
+        <v>5683.93</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>5419.2</v>
+      </c>
+      <c r="R9" s="2">
+        <v>6917.29</v>
+      </c>
+      <c r="S9" s="9">
+        <v>6728.85</v>
+      </c>
+      <c r="T9" s="2">
+        <v>6984.15</v>
+      </c>
+      <c r="U9" s="2">
+        <v>6677.03</v>
+      </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
+      <c r="B10" s="2">
+        <v>288</v>
+      </c>
+      <c r="C10" s="2">
+        <v>288</v>
+      </c>
+      <c r="D10" s="2">
+        <v>288</v>
+      </c>
+      <c r="E10" s="2">
+        <v>288</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1422.85</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1420.61</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1419.09</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1418.03</v>
+      </c>
+      <c r="J10" s="2">
+        <v>3579.98</v>
+      </c>
+      <c r="K10" s="9">
+        <v>3508.94</v>
+      </c>
+      <c r="L10" s="2">
+        <v>3612.09</v>
+      </c>
+      <c r="M10" s="2">
+        <v>3538.88</v>
+      </c>
+      <c r="N10" s="5">
+        <v>5958.78</v>
+      </c>
+      <c r="O10" s="9">
+        <v>5840.98</v>
+      </c>
+      <c r="P10" s="6">
+        <v>5974.08</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>5786.8</v>
+      </c>
+      <c r="R10" s="2">
+        <v>7407.25</v>
+      </c>
+      <c r="S10" s="9">
+        <v>7298.75</v>
+      </c>
+      <c r="T10" s="2">
+        <v>7388.34</v>
+      </c>
+      <c r="U10" s="2">
+        <v>7073.54</v>
+      </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
+      <c r="B11" s="2">
+        <v>288</v>
+      </c>
+      <c r="C11" s="2">
+        <v>288</v>
+      </c>
+      <c r="D11" s="2">
+        <v>288</v>
+      </c>
+      <c r="E11" s="2">
+        <v>282.25</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1457.73</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1464.03</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1449.91</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1449.82</v>
+      </c>
+      <c r="J11" s="2">
+        <v>3665.77</v>
+      </c>
+      <c r="K11" s="9">
+        <v>3630.66</v>
+      </c>
+      <c r="L11" s="2">
+        <v>3666.91</v>
+      </c>
+      <c r="M11" s="2">
+        <v>3628.95</v>
+      </c>
+      <c r="N11" s="5">
+        <v>6075.37</v>
+      </c>
+      <c r="O11" s="9">
+        <v>6009.09</v>
+      </c>
+      <c r="P11" s="6">
+        <v>6087.34</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>5950.3</v>
+      </c>
+      <c r="R11" s="2">
+        <v>7589.69</v>
+      </c>
+      <c r="S11" s="9">
+        <v>7532.33</v>
+      </c>
+      <c r="T11" s="2">
+        <v>7574.47</v>
+      </c>
+      <c r="U11" s="2">
+        <v>7401.15</v>
+      </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12">
@@ -1367,30 +1531,45 @@
     <mergeCell ref="R3:U3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started collecting music results and added direct to map implmentation
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-20" windowWidth="38020" windowHeight="21240"/>
+    <workbookView xWindow="2560" yWindow="0" windowWidth="34900" windowHeight="19500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Lyrics" sheetId="1" r:id="rId1"/>
+    <sheet name="Music" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="6">
   <si>
     <t>BL--Rthicke</t>
   </si>
@@ -37,12 +37,15 @@
   <si>
     <t>(%)</t>
   </si>
+  <si>
+    <t>For 2500</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,8 +61,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +103,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -94,10 +119,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -105,15 +136,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -503,36 +541,36 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="8">
         <v>0.2</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9">
         <v>0.4</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="7">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="8">
         <v>0.6</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="8">
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9">
         <v>0.8</v>
       </c>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="7">
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="8">
         <v>1</v>
       </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
     </row>
     <row r="4" spans="1:21">
       <c r="A4">
@@ -801,7 +839,7 @@
       <c r="B8" s="2">
         <v>240.49</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>231.17</v>
       </c>
       <c r="D8" s="2">
@@ -825,7 +863,7 @@
       <c r="J8" s="2">
         <v>2987.73</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="7">
         <v>2875.32</v>
       </c>
       <c r="L8" s="2">
@@ -837,7 +875,7 @@
       <c r="N8" s="5">
         <v>4910.5200000000004</v>
       </c>
-      <c r="O8" s="9">
+      <c r="O8" s="7">
         <v>4741.32</v>
       </c>
       <c r="P8" s="6">
@@ -890,7 +928,7 @@
       <c r="J9" s="2">
         <v>3415.66</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="7">
         <v>3227.09</v>
       </c>
       <c r="L9" s="2">
@@ -902,7 +940,7 @@
       <c r="N9" s="5">
         <v>5584.42</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="7">
         <v>5370.85</v>
       </c>
       <c r="P9" s="6">
@@ -914,7 +952,7 @@
       <c r="R9" s="2">
         <v>6917.29</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9" s="7">
         <v>6728.85</v>
       </c>
       <c r="T9" s="2">
@@ -946,7 +984,7 @@
       <c r="G10" s="6">
         <v>1420.61</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="7">
         <v>1419.09</v>
       </c>
       <c r="I10" s="5">
@@ -955,7 +993,7 @@
       <c r="J10" s="2">
         <v>3579.98</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="7">
         <v>3508.94</v>
       </c>
       <c r="L10" s="2">
@@ -967,7 +1005,7 @@
       <c r="N10" s="5">
         <v>5958.78</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="7">
         <v>5840.98</v>
       </c>
       <c r="P10" s="6">
@@ -979,7 +1017,7 @@
       <c r="R10" s="2">
         <v>7407.25</v>
       </c>
-      <c r="S10" s="9">
+      <c r="S10" s="7">
         <v>7298.75</v>
       </c>
       <c r="T10" s="2">
@@ -1020,7 +1058,7 @@
       <c r="J11" s="2">
         <v>3665.77</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="7">
         <v>3630.66</v>
       </c>
       <c r="L11" s="2">
@@ -1032,7 +1070,7 @@
       <c r="N11" s="5">
         <v>6075.37</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="7">
         <v>6009.09</v>
       </c>
       <c r="P11" s="6">
@@ -1044,7 +1082,7 @@
       <c r="R11" s="2">
         <v>7589.69</v>
       </c>
-      <c r="S11" s="9">
+      <c r="S11" s="7">
         <v>7532.33</v>
       </c>
       <c r="T11" s="2">
@@ -1542,13 +1580,408 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="8">
+        <v>1</v>
+      </c>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>28.42</v>
+      </c>
+      <c r="C3" s="7">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="D3" s="2">
+        <v>49.35</v>
+      </c>
+      <c r="E3" s="5">
+        <v>151.11000000000001</v>
+      </c>
+      <c r="F3" s="5">
+        <v>141.38999999999999</v>
+      </c>
+      <c r="G3" s="4">
+        <v>131.6</v>
+      </c>
+      <c r="H3" s="2">
+        <v>361.63</v>
+      </c>
+      <c r="I3" s="2">
+        <v>358.16</v>
+      </c>
+      <c r="J3" s="4">
+        <v>257.98</v>
+      </c>
+      <c r="K3" s="5">
+        <v>541.32000000000005</v>
+      </c>
+      <c r="L3" s="5">
+        <v>557.95000000000005</v>
+      </c>
+      <c r="M3" s="4">
+        <v>342.17</v>
+      </c>
+      <c r="N3" s="2">
+        <v>649.08000000000004</v>
+      </c>
+      <c r="O3" s="2">
+        <v>668.82</v>
+      </c>
+      <c r="P3" s="3">
+        <v>253.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>8349.9599999999991</v>
+      </c>
+      <c r="C4" s="10">
+        <v>9716.7800000000007</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12056.57</v>
+      </c>
+      <c r="E4" s="10">
+        <v>43652.53</v>
+      </c>
+      <c r="F4" s="6">
+        <v>47072.12</v>
+      </c>
+      <c r="G4" s="5">
+        <v>50791.97</v>
+      </c>
+      <c r="H4" s="2">
+        <v>98730.14</v>
+      </c>
+      <c r="I4" s="2">
+        <v>105318.23</v>
+      </c>
+      <c r="J4" s="4">
+        <v>93964.47</v>
+      </c>
+      <c r="K4" s="5">
+        <v>146614.85999999999</v>
+      </c>
+      <c r="L4" s="5">
+        <v>156276.4</v>
+      </c>
+      <c r="M4" s="4">
+        <v>99380.67</v>
+      </c>
+      <c r="N4" s="2">
+        <v>165994.16</v>
+      </c>
+      <c r="O4" s="2">
+        <v>171178.37</v>
+      </c>
+      <c r="P4" s="4">
+        <v>67279.14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2213.36</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2307.12</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2105.1799999999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4016.7</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4220.79</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3896.36</v>
+      </c>
+      <c r="H5" s="10">
+        <v>6029.02</v>
+      </c>
+      <c r="I5" s="2">
+        <v>6522.39</v>
+      </c>
+      <c r="J5" s="2">
+        <v>6235.01</v>
+      </c>
+      <c r="K5" s="10">
+        <v>8316.7199999999993</v>
+      </c>
+      <c r="L5" s="5">
+        <v>9277.18</v>
+      </c>
+      <c r="M5" s="6">
+        <v>8908.16</v>
+      </c>
+      <c r="N5" s="10">
+        <v>10661.94</v>
+      </c>
+      <c r="O5" s="2">
+        <v>11911.38</v>
+      </c>
+      <c r="P5" s="2">
+        <v>11897.15</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>